<commit_message>
add entities and sample files
</commit_message>
<xml_diff>
--- a/rd_connect_auto_template.xlsx
+++ b/rd_connect_auto_template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="rd_Disease Areas (ICD10)" sheetId="4" r:id="rId4"/>
+    <sheet name="rd_Disease_Areas_ICD10" sheetId="4" r:id="rId4"/>
     <sheet name="rd_address" sheetId="5" r:id="rId5"/>
     <sheet name="rd_basic_info" sheetId="6" r:id="rId6"/>
     <sheet name="rd_bb_accessibility" sheetId="7" r:id="rId7"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="167">
   <si>
     <t>name</t>
   </si>
@@ -66,7 +66,7 @@
     <t>description-en</t>
   </si>
   <si>
-    <t>Disease Areas (ICD10)</t>
+    <t>Disease_Areas_ICD10</t>
   </si>
   <si>
     <t>Directory</t>
@@ -141,6 +141,9 @@
     <t>rd_address</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
@@ -153,7 +156,10 @@
     <t>name of host institution</t>
   </si>
   <si>
-    <t>id_deseases</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>rd_diseases</t>
@@ -192,15 +198,12 @@
     <t>last activities</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>rd_reg_quality</t>
   </si>
   <si>
     <t>If_yes__specify</t>
   </si>
   <si>
-    <t>rd_reg_quality</t>
-  </si>
-  <si>
     <t>Accreditation_certification_program</t>
   </si>
   <si>
@@ -225,12 +228,12 @@
     <t>_fieldsDispla</t>
   </si>
   <si>
+    <t>rd_core</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>rd_core</t>
-  </si>
-  <si>
     <t>Additional_Imaging_available</t>
   </si>
   <si>
@@ -285,12 +288,12 @@
     <t>_fieldsDisplay</t>
   </si>
   <si>
+    <t>rd_contact</t>
+  </si>
+  <si>
     <t>last name</t>
   </si>
   <si>
-    <t>rd_contact</t>
-  </si>
-  <si>
     <t>first name</t>
   </si>
   <si>
@@ -330,12 +333,12 @@
     <t>Molecular_test_performed_to_ensure_sample_integrity</t>
   </si>
   <si>
+    <t>rd_Disease_Areas_ICD10</t>
+  </si>
+  <si>
     <t>Boolean4090</t>
   </si>
   <si>
-    <t>rd_Disease Areas (ICD10)</t>
-  </si>
-  <si>
     <t>Certain_conditions_originating_in_the_perinatal_period__P00-P96_</t>
   </si>
   <si>
@@ -387,12 +390,12 @@
     <t>others</t>
   </si>
   <si>
+    <t>rd_bb_accessibility</t>
+  </si>
+  <si>
     <t>Requirement_to_sign_a_material_transfer_agreement</t>
   </si>
   <si>
-    <t>rd_bb_accessibility</t>
-  </si>
-  <si>
     <t>Does_the_informed_consent_include_the_option_for_patients_to_withdraw_sample_at_any_time</t>
   </si>
   <si>
@@ -459,12 +462,15 @@
     <t>Other4838</t>
   </si>
   <si>
+    <t>id_bb_contribution</t>
+  </si>
+  <si>
+    <t>rd_bb_contribution</t>
+  </si>
+  <si>
     <t>Is_your_entire_sample_collection_available_for_the_RD-Connect_Catalogue</t>
   </si>
   <si>
-    <t>rd_bb_contribution</t>
-  </si>
-  <si>
     <t>If_not__please_specify_what_type_of_collections_can_be_publicly_available</t>
   </si>
   <si>
@@ -504,10 +510,10 @@
     <t>Do_you_use_a_Data_Access_Agreement_</t>
   </si>
   <si>
+    <t>rd_scientific publications</t>
+  </si>
+  <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>rd_scientific publications</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -892,72 +898,288 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1012,7 +1234,7 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1026,7 +1248,7 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1040,7 +1262,7 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1054,7 +1276,7 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1068,7 +1290,7 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1082,7 +1304,7 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1096,7 +1318,7 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1110,7 +1332,7 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1124,7 +1346,7 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1138,7 +1360,7 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1152,7 +1374,7 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1166,7 +1388,7 @@
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1177,7 +1399,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1237,13 +1459,16 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -1251,13 +1476,16 @@
       <c r="D3" t="s">
         <v>36</v>
       </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1265,13 +1493,16 @@
       <c r="D4" t="s">
         <v>36</v>
       </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -1279,13 +1510,16 @@
       <c r="D5" t="s">
         <v>36</v>
       </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -1293,131 +1527,167 @@
       <c r="D6" t="s">
         <v>36</v>
       </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
+      <c r="J8" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
+      <c r="H9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1431,85 +1701,109 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>52</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="H18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -1517,13 +1811,19 @@
       <c r="D22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
@@ -1531,13 +1831,16 @@
       <c r="D23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -1545,13 +1848,16 @@
       <c r="D24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -1559,13 +1865,16 @@
       <c r="D25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="H25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -1573,13 +1882,16 @@
       <c r="D26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="H26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1587,13 +1899,16 @@
       <c r="D27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1601,13 +1916,16 @@
       <c r="D28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -1615,41 +1933,50 @@
       <c r="D29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="H29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
       <c r="C31" t="s">
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>56</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
@@ -1657,13 +1984,19 @@
       <c r="D32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="H32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
@@ -1671,13 +2004,16 @@
       <c r="D33" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
         <v>35</v>
@@ -1685,13 +2021,16 @@
       <c r="D34" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="H34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
         <v>35</v>
@@ -1699,13 +2038,16 @@
       <c r="D35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
@@ -1713,13 +2055,16 @@
       <c r="D36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="H36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
@@ -1727,13 +2072,16 @@
       <c r="D37" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="H37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -1741,13 +2089,16 @@
       <c r="D38" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="H38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
         <v>35</v>
@@ -1755,13 +2106,16 @@
       <c r="D39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
@@ -1769,13 +2123,16 @@
       <c r="D40" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="H40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
         <v>35</v>
@@ -1783,13 +2140,16 @@
       <c r="D41" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
@@ -1797,13 +2157,16 @@
       <c r="D42" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="H42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
@@ -1811,13 +2174,16 @@
       <c r="D43" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="H43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
         <v>35</v>
@@ -1825,13 +2191,16 @@
       <c r="D44" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="H44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
@@ -1839,13 +2208,16 @@
       <c r="D45" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="H45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" t="s">
         <v>35</v>
@@ -1853,13 +2225,16 @@
       <c r="D46" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
@@ -1867,13 +2242,16 @@
       <c r="D47" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="H47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
         <v>35</v>
@@ -1881,55 +2259,67 @@
       <c r="D48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="H48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>66</v>
+      </c>
+      <c r="H49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="H50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
         <v>85</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>85</v>
       </c>
-      <c r="C49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" t="s">
         <v>35</v>
       </c>
       <c r="D51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>66</v>
+      </c>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
         <v>35</v>
@@ -1937,321 +2327,396 @@
       <c r="D52" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="H52" t="s">
+        <v>43</v>
+      </c>
+      <c r="J52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
         <v>35</v>
       </c>
       <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="H53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="H55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="H56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" t="s">
         <v>91</v>
       </c>
-      <c r="B54" t="s">
+      <c r="H57" t="s">
+        <v>43</v>
+      </c>
+      <c r="J57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" t="s">
         <v>91</v>
       </c>
-      <c r="C54" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+      <c r="H58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
         <v>92</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>92</v>
       </c>
-      <c r="C55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" t="s">
-        <v>35</v>
-      </c>
-      <c r="D56" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" t="s">
+        <v>91</v>
+      </c>
+      <c r="H62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>91</v>
+      </c>
+      <c r="H64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" t="s">
+        <v>91</v>
+      </c>
+      <c r="H65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" t="s">
+        <v>91</v>
+      </c>
+      <c r="H67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" t="s">
         <v>60</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B68" t="s">
         <v>60</v>
       </c>
-      <c r="C57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+      <c r="C68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" t="s">
+        <v>91</v>
+      </c>
+      <c r="H68" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
+      <c r="H69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" t="s">
+        <v>91</v>
+      </c>
+      <c r="H70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>99</v>
+      </c>
+      <c r="B71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" t="s">
+        <v>91</v>
+      </c>
+      <c r="H71" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
         <v>63</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B72" t="s">
         <v>63</v>
       </c>
-      <c r="C58" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>93</v>
-      </c>
-      <c r="B59" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" t="s">
-        <v>35</v>
-      </c>
-      <c r="D59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" t="s">
-        <v>35</v>
-      </c>
-      <c r="D64" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" t="s">
-        <v>35</v>
-      </c>
-      <c r="D65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>98</v>
-      </c>
-      <c r="B66" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" t="s">
-        <v>35</v>
-      </c>
-      <c r="D67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>99</v>
-      </c>
-      <c r="B68" t="s">
-        <v>99</v>
-      </c>
-      <c r="C68" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C69" t="s">
-        <v>35</v>
-      </c>
-      <c r="D69" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
+      <c r="C72" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" t="s">
+        <v>91</v>
+      </c>
+      <c r="H72" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" t="s">
         <v>100</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>100</v>
       </c>
-      <c r="C70" t="s">
-        <v>35</v>
-      </c>
-      <c r="D70" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" t="s">
-        <v>102</v>
-      </c>
-      <c r="C71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D71" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B72" t="s">
-        <v>103</v>
-      </c>
-      <c r="C72" t="s">
-        <v>35</v>
-      </c>
-      <c r="D72" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>104</v>
-      </c>
-      <c r="B73" t="s">
-        <v>104</v>
-      </c>
       <c r="C73" t="s">
         <v>35</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>91</v>
+      </c>
+      <c r="H73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>91</v>
+      </c>
+      <c r="H74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s">
         <v>35</v>
@@ -2259,13 +2724,19 @@
       <c r="D75" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="H75" t="s">
+        <v>43</v>
+      </c>
+      <c r="J75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C76" t="s">
         <v>35</v>
@@ -2273,13 +2744,16 @@
       <c r="D76" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="H76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C77" t="s">
         <v>35</v>
@@ -2287,13 +2761,16 @@
       <c r="D77" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="H77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B78" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C78" t="s">
         <v>35</v>
@@ -2301,13 +2778,16 @@
       <c r="D78" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="H78" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B79" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
         <v>35</v>
@@ -2315,13 +2795,16 @@
       <c r="D79" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="H79" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C80" t="s">
         <v>35</v>
@@ -2329,13 +2812,16 @@
       <c r="D80" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="H80" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
         <v>35</v>
@@ -2343,13 +2829,16 @@
       <c r="D81" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="H81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s">
         <v>35</v>
@@ -2357,13 +2846,16 @@
       <c r="D82" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="H82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
         <v>35</v>
@@ -2371,13 +2863,16 @@
       <c r="D83" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="H83" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B84" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C84" t="s">
         <v>35</v>
@@ -2385,13 +2880,16 @@
       <c r="D84" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="H84" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B85" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
         <v>35</v>
@@ -2399,13 +2897,16 @@
       <c r="D85" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="H85" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C86" t="s">
         <v>35</v>
@@ -2413,13 +2914,16 @@
       <c r="D86" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="H86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B87" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C87" t="s">
         <v>35</v>
@@ -2427,13 +2931,16 @@
       <c r="D87" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="H87" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
@@ -2441,97 +2948,118 @@
       <c r="D88" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="H88" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" t="s">
+        <v>35</v>
+      </c>
+      <c r="D89" t="s">
+        <v>101</v>
+      </c>
+      <c r="H89" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" t="s">
+        <v>35</v>
+      </c>
+      <c r="D90" t="s">
+        <v>101</v>
+      </c>
+      <c r="H90" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" t="s">
+        <v>101</v>
+      </c>
+      <c r="H91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" t="s">
+        <v>101</v>
+      </c>
+      <c r="H92" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" t="s">
         <v>119</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B93" t="s">
         <v>119</v>
       </c>
-      <c r="C89" t="s">
-        <v>35</v>
-      </c>
-      <c r="D89" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" t="s">
-        <v>121</v>
-      </c>
-      <c r="B90" t="s">
-        <v>121</v>
-      </c>
-      <c r="C90" t="s">
-        <v>35</v>
-      </c>
-      <c r="D90" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" t="s">
-        <v>122</v>
-      </c>
-      <c r="B91" t="s">
-        <v>122</v>
-      </c>
-      <c r="C91" t="s">
-        <v>35</v>
-      </c>
-      <c r="D91" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" t="s">
-        <v>123</v>
-      </c>
-      <c r="C92" t="s">
-        <v>35</v>
-      </c>
-      <c r="D92" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
-        <v>124</v>
-      </c>
-      <c r="B93" t="s">
-        <v>124</v>
-      </c>
       <c r="C93" t="s">
         <v>35</v>
       </c>
       <c r="D93" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>101</v>
+      </c>
+      <c r="H93" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
         <v>35</v>
       </c>
       <c r="D94" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>101</v>
+      </c>
+      <c r="H94" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="C95" t="s">
         <v>35</v>
@@ -2539,13 +3067,19 @@
       <c r="D95" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="H95" t="s">
+        <v>43</v>
+      </c>
+      <c r="J95" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C96" t="s">
         <v>35</v>
@@ -2553,13 +3087,16 @@
       <c r="D96" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="H96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C97" t="s">
         <v>35</v>
@@ -2567,13 +3104,16 @@
       <c r="D97" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="H97" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C98" t="s">
         <v>35</v>
@@ -2581,13 +3121,16 @@
       <c r="D98" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="H98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B99" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C99" t="s">
         <v>35</v>
@@ -2595,13 +3138,16 @@
       <c r="D99" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="H99" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C100" t="s">
         <v>35</v>
@@ -2609,13 +3155,16 @@
       <c r="D100" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="H100" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C101" t="s">
         <v>35</v>
@@ -2623,13 +3172,16 @@
       <c r="D101" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="H101" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B102" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C102" t="s">
         <v>35</v>
@@ -2637,13 +3189,16 @@
       <c r="D102" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="H102" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B103" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C103" t="s">
         <v>35</v>
@@ -2651,13 +3206,16 @@
       <c r="D103" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="H103" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B104" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C104" t="s">
         <v>35</v>
@@ -2665,13 +3223,16 @@
       <c r="D104" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="H104" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C105" t="s">
         <v>35</v>
@@ -2679,13 +3240,16 @@
       <c r="D105" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="H105" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B106" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C106" t="s">
         <v>35</v>
@@ -2693,13 +3257,16 @@
       <c r="D106" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="H106" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B107" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C107" t="s">
         <v>35</v>
@@ -2707,13 +3274,16 @@
       <c r="D107" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="H107" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B108" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C108" t="s">
         <v>35</v>
@@ -2721,13 +3291,16 @@
       <c r="D108" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="H108" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B109" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C109" t="s">
         <v>35</v>
@@ -2735,13 +3308,16 @@
       <c r="D109" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="H109" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B110" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C110" t="s">
         <v>35</v>
@@ -2749,13 +3325,16 @@
       <c r="D110" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="H110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B111" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C111" t="s">
         <v>35</v>
@@ -2763,13 +3342,16 @@
       <c r="D111" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="H111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="C112" t="s">
         <v>35</v>
@@ -2777,439 +3359,711 @@
       <c r="D112" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="H112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
+        <v>138</v>
+      </c>
+      <c r="B113" t="s">
+        <v>138</v>
+      </c>
+      <c r="C113" t="s">
+        <v>35</v>
+      </c>
+      <c r="D113" t="s">
+        <v>120</v>
+      </c>
+      <c r="H113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>139</v>
+      </c>
+      <c r="B114" t="s">
+        <v>139</v>
+      </c>
+      <c r="C114" t="s">
+        <v>35</v>
+      </c>
+      <c r="D114" t="s">
+        <v>120</v>
+      </c>
+      <c r="H114" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>140</v>
+      </c>
+      <c r="B115" t="s">
+        <v>140</v>
+      </c>
+      <c r="C115" t="s">
+        <v>35</v>
+      </c>
+      <c r="D115" t="s">
+        <v>120</v>
+      </c>
+      <c r="H115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" t="s">
+        <v>141</v>
+      </c>
+      <c r="C116" t="s">
+        <v>35</v>
+      </c>
+      <c r="D116" t="s">
+        <v>120</v>
+      </c>
+      <c r="H116" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+      <c r="B117" t="s">
+        <v>142</v>
+      </c>
+      <c r="C117" t="s">
+        <v>35</v>
+      </c>
+      <c r="D117" t="s">
+        <v>120</v>
+      </c>
+      <c r="H117" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
         <v>143</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B118" t="s">
         <v>143</v>
       </c>
-      <c r="C113" t="s">
-        <v>35</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C118" t="s">
+        <v>35</v>
+      </c>
+      <c r="D118" t="s">
+        <v>120</v>
+      </c>
+      <c r="H118" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>85</v>
+      </c>
+      <c r="B119" t="s">
+        <v>85</v>
+      </c>
+      <c r="C119" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119" t="s">
+        <v>120</v>
+      </c>
+      <c r="H119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" t="s">
+      <c r="B120" t="s">
+        <v>144</v>
+      </c>
+      <c r="C120" t="s">
+        <v>35</v>
+      </c>
+      <c r="D120" t="s">
         <v>145</v>
       </c>
-      <c r="B114" t="s">
+      <c r="H120" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B121" t="s">
+        <v>146</v>
+      </c>
+      <c r="C121" t="s">
+        <v>35</v>
+      </c>
+      <c r="D121" t="s">
         <v>145</v>
       </c>
-      <c r="C114" t="s">
-        <v>35</v>
-      </c>
-      <c r="D114" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" t="s">
-        <v>146</v>
-      </c>
-      <c r="B115" t="s">
-        <v>146</v>
-      </c>
-      <c r="C115" t="s">
-        <v>35</v>
-      </c>
-      <c r="D115" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" t="s">
+      <c r="H121" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
         <v>147</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B122" t="s">
         <v>147</v>
       </c>
-      <c r="C116" t="s">
-        <v>35</v>
-      </c>
-      <c r="D116" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" t="s">
+      <c r="C122" t="s">
+        <v>35</v>
+      </c>
+      <c r="D122" t="s">
+        <v>145</v>
+      </c>
+      <c r="H122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
         <v>148</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B123" t="s">
         <v>148</v>
       </c>
-      <c r="C117" t="s">
-        <v>35</v>
-      </c>
-      <c r="D117" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" t="s">
+      <c r="C123" t="s">
+        <v>35</v>
+      </c>
+      <c r="D123" t="s">
+        <v>145</v>
+      </c>
+      <c r="H123" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
         <v>149</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B124" t="s">
         <v>149</v>
       </c>
-      <c r="C118" t="s">
-        <v>35</v>
-      </c>
-      <c r="D118" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" t="s">
+      <c r="C124" t="s">
+        <v>35</v>
+      </c>
+      <c r="D124" t="s">
+        <v>145</v>
+      </c>
+      <c r="H124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
         <v>150</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B125" t="s">
         <v>150</v>
       </c>
-      <c r="C119" t="s">
-        <v>35</v>
-      </c>
-      <c r="D119" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" t="s">
+      <c r="C125" t="s">
+        <v>35</v>
+      </c>
+      <c r="D125" t="s">
+        <v>145</v>
+      </c>
+      <c r="H125" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
         <v>151</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B126" t="s">
         <v>151</v>
       </c>
-      <c r="C120" t="s">
-        <v>35</v>
-      </c>
-      <c r="D120" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" t="s">
+      <c r="C126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D126" t="s">
+        <v>145</v>
+      </c>
+      <c r="H126" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
         <v>152</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B127" t="s">
         <v>152</v>
       </c>
-      <c r="C121" t="s">
-        <v>35</v>
-      </c>
-      <c r="D121" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" t="s">
-        <v>84</v>
-      </c>
-      <c r="B122" t="s">
-        <v>84</v>
-      </c>
-      <c r="C122" t="s">
-        <v>35</v>
-      </c>
-      <c r="D122" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" t="s">
-        <v>122</v>
-      </c>
-      <c r="B123" t="s">
-        <v>122</v>
-      </c>
-      <c r="C123" t="s">
-        <v>35</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C127" t="s">
+        <v>35</v>
+      </c>
+      <c r="D127" t="s">
+        <v>145</v>
+      </c>
+      <c r="H127" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" t="s">
+      <c r="B128" t="s">
+        <v>153</v>
+      </c>
+      <c r="C128" t="s">
+        <v>35</v>
+      </c>
+      <c r="D128" t="s">
+        <v>145</v>
+      </c>
+      <c r="H128" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" t="s">
+        <v>154</v>
+      </c>
+      <c r="C129" t="s">
+        <v>35</v>
+      </c>
+      <c r="D129" t="s">
+        <v>145</v>
+      </c>
+      <c r="H129" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" t="s">
+        <v>85</v>
+      </c>
+      <c r="B130" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" t="s">
+        <v>35</v>
+      </c>
+      <c r="D130" t="s">
+        <v>145</v>
+      </c>
+      <c r="H130" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="A131" t="s">
+        <v>42</v>
+      </c>
+      <c r="B131" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" t="s">
+        <v>35</v>
+      </c>
+      <c r="D131" t="s">
+        <v>155</v>
+      </c>
+      <c r="H131" t="s">
+        <v>43</v>
+      </c>
+      <c r="J131" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="A132" t="s">
         <v>123</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B132" t="s">
         <v>123</v>
       </c>
-      <c r="C124" t="s">
-        <v>35</v>
-      </c>
-      <c r="D124" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
-        <v>154</v>
-      </c>
-      <c r="B125" t="s">
-        <v>154</v>
-      </c>
-      <c r="C125" t="s">
-        <v>35</v>
-      </c>
-      <c r="D125" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
+      <c r="C132" t="s">
+        <v>35</v>
+      </c>
+      <c r="D132" t="s">
+        <v>155</v>
+      </c>
+      <c r="H132" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="A133" t="s">
         <v>124</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B133" t="s">
         <v>124</v>
       </c>
-      <c r="C126" t="s">
-        <v>35</v>
-      </c>
-      <c r="D126" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" t="s">
+      <c r="C133" t="s">
+        <v>35</v>
+      </c>
+      <c r="D133" t="s">
         <v>155</v>
       </c>
-      <c r="B127" t="s">
+      <c r="H133" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
+      <c r="A134" t="s">
+        <v>156</v>
+      </c>
+      <c r="B134" t="s">
+        <v>156</v>
+      </c>
+      <c r="C134" t="s">
+        <v>35</v>
+      </c>
+      <c r="D134" t="s">
         <v>155</v>
       </c>
-      <c r="C127" t="s">
-        <v>35</v>
-      </c>
-      <c r="D127" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="A128" t="s">
-        <v>127</v>
-      </c>
-      <c r="B128" t="s">
-        <v>127</v>
-      </c>
-      <c r="C128" t="s">
-        <v>35</v>
-      </c>
-      <c r="D128" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="A129" t="s">
-        <v>134</v>
-      </c>
-      <c r="B129" t="s">
-        <v>134</v>
-      </c>
-      <c r="C129" t="s">
-        <v>35</v>
-      </c>
-      <c r="D129" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" t="s">
-        <v>156</v>
-      </c>
-      <c r="B130" t="s">
-        <v>156</v>
-      </c>
-      <c r="C130" t="s">
-        <v>35</v>
-      </c>
-      <c r="D130" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" t="s">
-        <v>136</v>
-      </c>
-      <c r="B131" t="s">
-        <v>136</v>
-      </c>
-      <c r="C131" t="s">
-        <v>35</v>
-      </c>
-      <c r="D131" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132" t="s">
+      <c r="H134" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
+      <c r="A135" t="s">
+        <v>125</v>
+      </c>
+      <c r="B135" t="s">
+        <v>125</v>
+      </c>
+      <c r="C135" t="s">
+        <v>35</v>
+      </c>
+      <c r="D135" t="s">
+        <v>155</v>
+      </c>
+      <c r="H135" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" t="s">
         <v>157</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B136" t="s">
         <v>157</v>
       </c>
-      <c r="C132" t="s">
-        <v>35</v>
-      </c>
-      <c r="D132" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" t="s">
+      <c r="C136" t="s">
+        <v>35</v>
+      </c>
+      <c r="D136" t="s">
+        <v>155</v>
+      </c>
+      <c r="H136" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
+      <c r="A137" t="s">
+        <v>128</v>
+      </c>
+      <c r="B137" t="s">
+        <v>128</v>
+      </c>
+      <c r="C137" t="s">
+        <v>35</v>
+      </c>
+      <c r="D137" t="s">
+        <v>155</v>
+      </c>
+      <c r="H137" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="A138" t="s">
+        <v>135</v>
+      </c>
+      <c r="B138" t="s">
+        <v>135</v>
+      </c>
+      <c r="C138" t="s">
+        <v>35</v>
+      </c>
+      <c r="D138" t="s">
+        <v>155</v>
+      </c>
+      <c r="H138" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" t="s">
+        <v>158</v>
+      </c>
+      <c r="B139" t="s">
+        <v>158</v>
+      </c>
+      <c r="C139" t="s">
+        <v>35</v>
+      </c>
+      <c r="D139" t="s">
+        <v>155</v>
+      </c>
+      <c r="H139" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="A140" t="s">
         <v>137</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B140" t="s">
         <v>137</v>
       </c>
-      <c r="C133" t="s">
-        <v>35</v>
-      </c>
-      <c r="D133" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" t="s">
-        <v>139</v>
-      </c>
-      <c r="B134" t="s">
-        <v>139</v>
-      </c>
-      <c r="C134" t="s">
-        <v>35</v>
-      </c>
-      <c r="D134" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" t="s">
-        <v>142</v>
-      </c>
-      <c r="B135" t="s">
-        <v>142</v>
-      </c>
-      <c r="C135" t="s">
-        <v>35</v>
-      </c>
-      <c r="D135" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" t="s">
-        <v>84</v>
-      </c>
-      <c r="B136" t="s">
-        <v>84</v>
-      </c>
-      <c r="C136" t="s">
-        <v>35</v>
-      </c>
-      <c r="D136" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" t="s">
-        <v>158</v>
-      </c>
-      <c r="B137" t="s">
-        <v>158</v>
-      </c>
-      <c r="C137" t="s">
-        <v>35</v>
-      </c>
-      <c r="D137" t="s">
+      <c r="C140" t="s">
+        <v>35</v>
+      </c>
+      <c r="D140" t="s">
+        <v>155</v>
+      </c>
+      <c r="H140" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" t="s">
+      <c r="B141" t="s">
+        <v>159</v>
+      </c>
+      <c r="C141" t="s">
+        <v>35</v>
+      </c>
+      <c r="D141" t="s">
+        <v>155</v>
+      </c>
+      <c r="H141" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" t="s">
+        <v>138</v>
+      </c>
+      <c r="C142" t="s">
+        <v>35</v>
+      </c>
+      <c r="D142" t="s">
+        <v>155</v>
+      </c>
+      <c r="H142" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="A143" t="s">
+        <v>140</v>
+      </c>
+      <c r="B143" t="s">
+        <v>140</v>
+      </c>
+      <c r="C143" t="s">
+        <v>35</v>
+      </c>
+      <c r="D143" t="s">
+        <v>155</v>
+      </c>
+      <c r="H143" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>143</v>
+      </c>
+      <c r="C144" t="s">
+        <v>35</v>
+      </c>
+      <c r="D144" t="s">
+        <v>155</v>
+      </c>
+      <c r="H144" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" t="s">
+        <v>85</v>
+      </c>
+      <c r="B145" t="s">
+        <v>85</v>
+      </c>
+      <c r="C145" t="s">
+        <v>35</v>
+      </c>
+      <c r="D145" t="s">
+        <v>155</v>
+      </c>
+      <c r="H145" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" t="s">
+        <v>42</v>
+      </c>
+      <c r="B146" t="s">
+        <v>42</v>
+      </c>
+      <c r="C146" t="s">
+        <v>35</v>
+      </c>
+      <c r="D146" t="s">
         <v>160</v>
       </c>
-      <c r="B138" t="s">
+      <c r="H146" t="s">
+        <v>43</v>
+      </c>
+      <c r="J146" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" t="s">
+        <v>161</v>
+      </c>
+      <c r="B147" t="s">
+        <v>161</v>
+      </c>
+      <c r="C147" t="s">
+        <v>35</v>
+      </c>
+      <c r="D147" t="s">
         <v>160</v>
       </c>
-      <c r="C138" t="s">
-        <v>35</v>
-      </c>
-      <c r="D138" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" t="s">
-        <v>161</v>
-      </c>
-      <c r="B139" t="s">
-        <v>161</v>
-      </c>
-      <c r="C139" t="s">
-        <v>35</v>
-      </c>
-      <c r="D139" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140" t="s">
+      <c r="H147" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
+      <c r="A148" t="s">
         <v>162</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B148" t="s">
         <v>162</v>
       </c>
-      <c r="C140" t="s">
-        <v>35</v>
-      </c>
-      <c r="D140" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141" t="s">
+      <c r="C148" t="s">
+        <v>35</v>
+      </c>
+      <c r="D148" t="s">
+        <v>160</v>
+      </c>
+      <c r="H148" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
+      <c r="A149" t="s">
         <v>163</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B149" t="s">
         <v>163</v>
       </c>
-      <c r="C141" t="s">
-        <v>35</v>
-      </c>
-      <c r="D141" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" t="s">
+      <c r="C149" t="s">
+        <v>35</v>
+      </c>
+      <c r="D149" t="s">
+        <v>160</v>
+      </c>
+      <c r="H149" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="A150" t="s">
         <v>164</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B150" t="s">
         <v>164</v>
       </c>
-      <c r="C142" t="s">
-        <v>35</v>
-      </c>
-      <c r="D142" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" t="s">
-        <v>84</v>
-      </c>
-      <c r="B143" t="s">
-        <v>84</v>
-      </c>
-      <c r="C143" t="s">
-        <v>35</v>
-      </c>
-      <c r="D143" t="s">
-        <v>159</v>
+      <c r="C150" t="s">
+        <v>35</v>
+      </c>
+      <c r="D150" t="s">
+        <v>160</v>
+      </c>
+      <c r="H150" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="A151" t="s">
+        <v>165</v>
+      </c>
+      <c r="B151" t="s">
+        <v>165</v>
+      </c>
+      <c r="C151" t="s">
+        <v>35</v>
+      </c>
+      <c r="D151" t="s">
+        <v>160</v>
+      </c>
+      <c r="H151" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="A152" t="s">
+        <v>166</v>
+      </c>
+      <c r="B152" t="s">
+        <v>166</v>
+      </c>
+      <c r="C152" t="s">
+        <v>35</v>
+      </c>
+      <c r="D152" t="s">
+        <v>160</v>
+      </c>
+      <c r="H152" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" t="s">
+        <v>85</v>
+      </c>
+      <c r="B153" t="s">
+        <v>85</v>
+      </c>
+      <c r="C153" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" t="s">
+        <v>160</v>
+      </c>
+      <c r="H153" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3219,72 +4073,348 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" t="s">
+        <v>140</v>
+      </c>
+      <c r="V1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W1" t="s">
+        <v>142</v>
+      </c>
+      <c r="X1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added clean_EMX_func for removal of unallowed chars
</commit_message>
<xml_diff>
--- a/rd_connect_auto_template.xlsx
+++ b/rd_connect_auto_template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="166">
   <si>
     <t>name</t>
   </si>
@@ -462,10 +462,10 @@
     <t>Other4838</t>
   </si>
   <si>
+    <t>rd_bb_contribution</t>
+  </si>
+  <si>
     <t>Is_your_entire_sample_collection_available_for_the_RD-Connect_Catalogue</t>
-  </si>
-  <si>
-    <t>rd_bb_contribution</t>
   </si>
   <si>
     <t>If_not__please_specify_what_type_of_collections_can_be_publicly_available</t>
@@ -1396,7 +1396,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M152"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3360,7 +3360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>138</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>139</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>140</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>141</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>142</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>143</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -3479,154 +3479,157 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
+        <v>42</v>
+      </c>
+      <c r="B120" t="s">
+        <v>42</v>
+      </c>
+      <c r="C120" t="s">
+        <v>35</v>
+      </c>
+      <c r="D120" t="s">
         <v>144</v>
       </c>
-      <c r="B120" t="s">
+      <c r="H120" t="s">
+        <v>43</v>
+      </c>
+      <c r="J120" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B121" t="s">
+        <v>145</v>
+      </c>
+      <c r="C121" t="s">
+        <v>35</v>
+      </c>
+      <c r="D121" t="s">
         <v>144</v>
       </c>
-      <c r="C120" t="s">
-        <v>35</v>
-      </c>
-      <c r="D120" t="s">
-        <v>145</v>
-      </c>
-      <c r="H120" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" t="s">
+      <c r="H121" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" t="s">
         <v>146</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>146</v>
       </c>
-      <c r="C121" t="s">
-        <v>35</v>
-      </c>
-      <c r="D121" t="s">
-        <v>145</v>
-      </c>
-      <c r="H121" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
-      <c r="A122" t="s">
+      <c r="C122" t="s">
+        <v>35</v>
+      </c>
+      <c r="D122" t="s">
+        <v>144</v>
+      </c>
+      <c r="H122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" t="s">
         <v>147</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>147</v>
       </c>
-      <c r="C122" t="s">
-        <v>35</v>
-      </c>
-      <c r="D122" t="s">
-        <v>145</v>
-      </c>
-      <c r="H122" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
-      <c r="A123" t="s">
+      <c r="C123" t="s">
+        <v>35</v>
+      </c>
+      <c r="D123" t="s">
+        <v>144</v>
+      </c>
+      <c r="H123" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" t="s">
         <v>148</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>148</v>
       </c>
-      <c r="C123" t="s">
-        <v>35</v>
-      </c>
-      <c r="D123" t="s">
-        <v>145</v>
-      </c>
-      <c r="H123" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
-      <c r="A124" t="s">
+      <c r="C124" t="s">
+        <v>35</v>
+      </c>
+      <c r="D124" t="s">
+        <v>144</v>
+      </c>
+      <c r="H124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" t="s">
         <v>149</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>149</v>
       </c>
-      <c r="C124" t="s">
-        <v>35</v>
-      </c>
-      <c r="D124" t="s">
-        <v>145</v>
-      </c>
-      <c r="H124" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
-      <c r="A125" t="s">
+      <c r="C125" t="s">
+        <v>35</v>
+      </c>
+      <c r="D125" t="s">
+        <v>144</v>
+      </c>
+      <c r="H125" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" t="s">
         <v>150</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>150</v>
       </c>
-      <c r="C125" t="s">
-        <v>35</v>
-      </c>
-      <c r="D125" t="s">
-        <v>145</v>
-      </c>
-      <c r="H125" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
-      <c r="A126" t="s">
+      <c r="C126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D126" t="s">
+        <v>144</v>
+      </c>
+      <c r="H126" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" t="s">
         <v>151</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>151</v>
       </c>
-      <c r="C126" t="s">
-        <v>35</v>
-      </c>
-      <c r="D126" t="s">
-        <v>145</v>
-      </c>
-      <c r="H126" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
-      <c r="A127" t="s">
+      <c r="C127" t="s">
+        <v>35</v>
+      </c>
+      <c r="D127" t="s">
+        <v>144</v>
+      </c>
+      <c r="H127" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" t="s">
         <v>152</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>152</v>
       </c>
-      <c r="C127" t="s">
-        <v>35</v>
-      </c>
-      <c r="D127" t="s">
-        <v>145</v>
-      </c>
-      <c r="H127" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" t="s">
-        <v>153</v>
-      </c>
-      <c r="B128" t="s">
-        <v>153</v>
-      </c>
       <c r="C128" t="s">
         <v>35</v>
       </c>
       <c r="D128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H128" t="s">
         <v>37</v>
@@ -3634,16 +3637,16 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="B129" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="C129" t="s">
         <v>35</v>
       </c>
       <c r="D129" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H129" t="s">
         <v>37</v>
@@ -3651,30 +3654,27 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B130" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C130" t="s">
         <v>35</v>
       </c>
       <c r="D130" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H130" t="s">
-        <v>43</v>
-      </c>
-      <c r="J130" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="C131" t="s">
         <v>35</v>
@@ -3683,15 +3683,18 @@
         <v>154</v>
       </c>
       <c r="H131" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="J131" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C132" t="s">
         <v>35</v>
@@ -3705,10 +3708,10 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="B133" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="C133" t="s">
         <v>35</v>
@@ -3722,10 +3725,10 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="C134" t="s">
         <v>35</v>
@@ -3739,10 +3742,10 @@
     </row>
     <row r="135" spans="1:10">
       <c r="A135" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C135" t="s">
         <v>35</v>
@@ -3756,10 +3759,10 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="B136" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="C136" t="s">
         <v>35</v>
@@ -3773,10 +3776,10 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C137" t="s">
         <v>35</v>
@@ -3790,10 +3793,10 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="C138" t="s">
         <v>35</v>
@@ -3807,10 +3810,10 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C139" t="s">
         <v>35</v>
@@ -3824,10 +3827,10 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C140" t="s">
         <v>35</v>
@@ -3841,10 +3844,10 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B141" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C141" t="s">
         <v>35</v>
@@ -3858,10 +3861,10 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C142" t="s">
         <v>35</v>
@@ -3875,10 +3878,10 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C143" t="s">
         <v>35</v>
@@ -3892,10 +3895,10 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="C144" t="s">
         <v>35</v>
@@ -3909,30 +3912,27 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B145" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C145" t="s">
         <v>35</v>
       </c>
       <c r="D145" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H145" t="s">
-        <v>43</v>
-      </c>
-      <c r="J145" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="C146" t="s">
         <v>35</v>
@@ -3941,15 +3941,18 @@
         <v>159</v>
       </c>
       <c r="H146" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="J146" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C147" t="s">
         <v>35</v>
@@ -3963,10 +3966,10 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C148" t="s">
         <v>35</v>
@@ -3980,10 +3983,10 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C149" t="s">
         <v>35</v>
@@ -3997,10 +4000,10 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C150" t="s">
         <v>35</v>
@@ -4014,10 +4017,10 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C151" t="s">
         <v>35</v>
@@ -4031,10 +4034,10 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B152" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="C152" t="s">
         <v>35</v>
@@ -4043,6 +4046,23 @@
         <v>159</v>
       </c>
       <c r="H152" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" t="s">
+        <v>85</v>
+      </c>
+      <c r="B153" t="s">
+        <v>85</v>
+      </c>
+      <c r="C153" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" t="s">
+        <v>159</v>
+      </c>
+      <c r="H153" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4284,41 +4304,44 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>148</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>152</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>153</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add some test files
</commit_message>
<xml_diff>
--- a/rd_connect_auto_template.xlsx
+++ b/rd_connect_auto_template.xlsx
@@ -16,20 +16,21 @@
     <sheet name="rd_basic_info" sheetId="7" r:id="rId7"/>
     <sheet name="rd_bb_accessibility" sheetId="8" r:id="rId8"/>
     <sheet name="rd_bb_contribution" sheetId="9" r:id="rId9"/>
-    <sheet name="rd_bb_quality" sheetId="10" r:id="rId10"/>
-    <sheet name="rd_contact" sheetId="11" r:id="rId11"/>
-    <sheet name="rd_core" sheetId="12" r:id="rId12"/>
-    <sheet name="rd_diseases" sheetId="13" r:id="rId13"/>
-    <sheet name="rd_reg_accessibility" sheetId="14" r:id="rId14"/>
-    <sheet name="rd_reg_quality" sheetId="15" r:id="rId15"/>
-    <sheet name="rd_url" sheetId="16" r:id="rId16"/>
+    <sheet name="rd_bb_core" sheetId="10" r:id="rId10"/>
+    <sheet name="rd_bb_quality" sheetId="11" r:id="rId11"/>
+    <sheet name="rd_contacts" sheetId="12" r:id="rId12"/>
+    <sheet name="rd_core" sheetId="13" r:id="rId13"/>
+    <sheet name="rd_diseases" sheetId="14" r:id="rId14"/>
+    <sheet name="rd_reg_accessibility" sheetId="15" r:id="rId15"/>
+    <sheet name="rd_reg_quality" sheetId="16" r:id="rId16"/>
+    <sheet name="rd_url" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="181">
   <si>
     <t>name</t>
   </si>
@@ -46,7 +47,7 @@
     <t>rd</t>
   </si>
   <si>
-    <t>RD-Connect Auto Template</t>
+    <t>rd_connect_auto_template</t>
   </si>
   <si>
     <t>package</t>
@@ -70,9 +71,6 @@
     <t>Disease Areas (ICD10)</t>
   </si>
   <si>
-    <t>Directory</t>
-  </si>
-  <si>
     <t>PostgreSQL</t>
   </si>
   <si>
@@ -91,10 +89,13 @@
     <t>bb_contribution</t>
   </si>
   <si>
+    <t>bb_core</t>
+  </si>
+  <si>
     <t>bb_quality</t>
   </si>
   <si>
-    <t>contact</t>
+    <t>contacts</t>
   </si>
   <si>
     <t>core</t>
@@ -166,6 +167,9 @@
     <t>ID</t>
   </si>
   <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
@@ -232,7 +236,7 @@
     <t>Standardized_case-inclusion_and-exclusion_criteria</t>
   </si>
   <si>
-    <t>_fieldsDispla</t>
+    <t>_fieldsDisplay</t>
   </si>
   <si>
     <t>rd_core</t>
@@ -292,10 +296,7 @@
     <t>Additional_networks_inventories</t>
   </si>
   <si>
-    <t>_fieldsDisplay</t>
-  </si>
-  <si>
-    <t>rd_contact</t>
+    <t>rd_contacts</t>
   </si>
   <si>
     <t>last name</t>
@@ -307,6 +308,9 @@
     <t>email</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>main</t>
   </si>
   <si>
@@ -536,6 +540,39 @@
   </si>
   <si>
     <t>rd_url</t>
+  </si>
+  <si>
+    <t>rd_bb_core</t>
+  </si>
+  <si>
+    <t>Additional_Biomaterial_available</t>
+  </si>
+  <si>
+    <t>Additional_Origin_of_collection</t>
+  </si>
+  <si>
+    <t>How_many_RD_are_in_the_registry_biobank</t>
+  </si>
+  <si>
+    <t>Use_of_collection</t>
+  </si>
+  <si>
+    <t>Origin_of_collection</t>
+  </si>
+  <si>
+    <t>Additional_Biomaterial_prepared</t>
+  </si>
+  <si>
+    <t>Biomaterial_Available</t>
+  </si>
+  <si>
+    <t>Percentage_of_rare_diseases_in_your_registry_biobank</t>
+  </si>
+  <si>
+    <t>Biomaterial_prepared</t>
+  </si>
+  <si>
+    <t>Additional_Use_of_collection</t>
   </si>
 </sst>
 </file>
@@ -905,6 +942,108 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -913,94 +1052,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
       <c r="R1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1009,6 +1115,42 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U1"/>
   <sheetViews>
@@ -1018,67 +1160,67 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="U1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1096,31 +1238,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -1138,52 +1280,52 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="P1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -1201,37 +1343,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1252,7 +1394,7 @@
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
@@ -1265,7 +1407,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1311,178 +1453,192 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
         <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
         <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
         <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
         <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
         <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>14</v>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1492,7 +1648,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M168"/>
+  <dimension ref="A1:M198"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1654,19 +1810,22 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -1680,16 +1839,16 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
         <v>38</v>
@@ -1706,27 +1865,30 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -1734,16 +1896,16 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1751,16 +1913,16 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -1768,16 +1930,16 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -1794,7 +1956,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -1802,16 +1964,16 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>
@@ -1819,16 +1981,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
         <v>38</v>
@@ -1836,16 +1998,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
         <v>38</v>
@@ -1853,36 +2015,39 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="J20" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
       </c>
       <c r="H21" t="s">
         <v>38</v>
@@ -1890,16 +2055,16 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
         <v>38</v>
@@ -1916,7 +2081,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
         <v>38</v>
@@ -1933,7 +2098,7 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
@@ -1941,16 +2106,16 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
@@ -1967,27 +2132,30 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
       </c>
       <c r="H27" t="s">
         <v>38</v>
@@ -1995,16 +2163,16 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H28" t="s">
         <v>38</v>
@@ -2012,16 +2180,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H29" t="s">
         <v>38</v>
@@ -2029,16 +2197,16 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H30" t="s">
         <v>38</v>
@@ -2046,16 +2214,16 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H31" t="s">
         <v>38</v>
@@ -2063,16 +2231,16 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H32" t="s">
         <v>38</v>
@@ -2080,16 +2248,16 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H33" t="s">
         <v>38</v>
@@ -2097,16 +2265,16 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H34" t="s">
         <v>38</v>
@@ -2114,16 +2282,16 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H35" t="s">
         <v>38</v>
@@ -2131,16 +2299,16 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H36" t="s">
         <v>38</v>
@@ -2157,27 +2325,30 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
       </c>
       <c r="H37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
         <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>68</v>
       </c>
       <c r="H38" t="s">
         <v>38</v>
@@ -2185,16 +2356,16 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H39" t="s">
         <v>38</v>
@@ -2202,16 +2373,16 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
         <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H40" t="s">
         <v>38</v>
@@ -2219,16 +2390,16 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
         <v>36</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H41" t="s">
         <v>38</v>
@@ -2236,16 +2407,16 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H42" t="s">
         <v>38</v>
@@ -2253,16 +2424,16 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
         <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H43" t="s">
         <v>38</v>
@@ -2270,16 +2441,16 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H44" t="s">
         <v>38</v>
@@ -2287,16 +2458,16 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
         <v>36</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H45" t="s">
         <v>38</v>
@@ -2304,16 +2475,16 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
         <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H46" t="s">
         <v>38</v>
@@ -2321,16 +2492,16 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
         <v>36</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H47" t="s">
         <v>38</v>
@@ -2338,16 +2509,16 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
         <v>36</v>
       </c>
       <c r="D48" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H48" t="s">
         <v>38</v>
@@ -2355,16 +2526,16 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
         <v>36</v>
       </c>
       <c r="D49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H49" t="s">
         <v>38</v>
@@ -2372,16 +2543,16 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C50" t="s">
         <v>36</v>
       </c>
       <c r="D50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H50" t="s">
         <v>38</v>
@@ -2389,16 +2560,16 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
         <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>
@@ -2406,16 +2577,16 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C52" t="s">
         <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H52" t="s">
         <v>38</v>
@@ -2423,16 +2594,16 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C53" t="s">
         <v>36</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H53" t="s">
         <v>38</v>
@@ -2440,16 +2611,16 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
         <v>36</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H54" t="s">
         <v>38</v>
@@ -2457,16 +2628,16 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C55" t="s">
         <v>36</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H55" t="s">
         <v>38</v>
@@ -2474,16 +2645,16 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
         <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H56" t="s">
         <v>38</v>
@@ -2491,10 +2662,10 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
         <v>36</v>
@@ -2519,11 +2690,14 @@
       <c r="D58" t="s">
         <v>88</v>
       </c>
+      <c r="E58" t="s">
+        <v>45</v>
+      </c>
       <c r="H58" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J58" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2596,16 +2770,16 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
         <v>36</v>
       </c>
       <c r="D63" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H63" t="s">
         <v>38</v>
@@ -2613,59 +2787,62 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>36</v>
+      </c>
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+      <c r="H64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
         <v>44</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>44</v>
       </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" t="s">
-        <v>93</v>
-      </c>
-      <c r="H64" t="s">
+      <c r="C65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" t="s">
         <v>45</v>
       </c>
-      <c r="J64" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" t="s">
-        <v>36</v>
-      </c>
-      <c r="D65" t="s">
-        <v>93</v>
-      </c>
       <c r="H65" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>46</v>
+      </c>
+      <c r="J65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" t="s">
         <v>94</v>
       </c>
-      <c r="B66" t="s">
-        <v>94</v>
-      </c>
-      <c r="C66" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" t="s">
-        <v>93</v>
-      </c>
       <c r="H66" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -2676,81 +2853,81 @@
         <v>36</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
         <v>36</v>
       </c>
       <c r="D68" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H68" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C69" t="s">
         <v>36</v>
       </c>
       <c r="D69" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C70" t="s">
         <v>36</v>
       </c>
       <c r="D70" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
         <v>36</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>97</v>
       </c>
@@ -2761,13 +2938,13 @@
         <v>36</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H72" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -2778,13 +2955,13 @@
         <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H73" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>99</v>
       </c>
@@ -2795,109 +2972,109 @@
         <v>36</v>
       </c>
       <c r="D74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H74" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="C75" t="s">
         <v>36</v>
       </c>
       <c r="D75" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H75" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C76" t="s">
         <v>36</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H76" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C77" t="s">
         <v>36</v>
       </c>
       <c r="D77" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H77" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="C78" t="s">
         <v>36</v>
       </c>
       <c r="D78" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H78" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="C79" t="s">
         <v>36</v>
       </c>
       <c r="D79" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H79" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
         <v>36</v>
       </c>
       <c r="D80" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H80" t="s">
         <v>38</v>
@@ -2905,16 +3082,16 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
         <v>36</v>
       </c>
       <c r="D81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H81" t="s">
         <v>38</v>
@@ -2922,16 +3099,16 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B82" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
         <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="H82" t="s">
         <v>38</v>
@@ -2939,39 +3116,42 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C83" t="s">
         <v>36</v>
       </c>
       <c r="D83" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H83" t="s">
-        <v>45</v>
-      </c>
-      <c r="J83" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" t="s">
+        <v>36</v>
+      </c>
+      <c r="D84" t="s">
         <v>104</v>
       </c>
-      <c r="B84" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" t="s">
-        <v>36</v>
-      </c>
-      <c r="D84" t="s">
-        <v>103</v>
+      <c r="E84" t="s">
+        <v>45</v>
       </c>
       <c r="H84" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="J84" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -2985,7 +3165,7 @@
         <v>36</v>
       </c>
       <c r="D85" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H85" t="s">
         <v>38</v>
@@ -3002,7 +3182,7 @@
         <v>36</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H86" t="s">
         <v>38</v>
@@ -3019,7 +3199,7 @@
         <v>36</v>
       </c>
       <c r="D87" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H87" t="s">
         <v>38</v>
@@ -3036,7 +3216,7 @@
         <v>36</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H88" t="s">
         <v>38</v>
@@ -3053,7 +3233,7 @@
         <v>36</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H89" t="s">
         <v>38</v>
@@ -3070,7 +3250,7 @@
         <v>36</v>
       </c>
       <c r="D90" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H90" t="s">
         <v>38</v>
@@ -3087,7 +3267,7 @@
         <v>36</v>
       </c>
       <c r="D91" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H91" t="s">
         <v>38</v>
@@ -3104,7 +3284,7 @@
         <v>36</v>
       </c>
       <c r="D92" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H92" t="s">
         <v>38</v>
@@ -3121,7 +3301,7 @@
         <v>36</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H93" t="s">
         <v>38</v>
@@ -3138,7 +3318,7 @@
         <v>36</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H94" t="s">
         <v>38</v>
@@ -3155,7 +3335,7 @@
         <v>36</v>
       </c>
       <c r="D95" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H95" t="s">
         <v>38</v>
@@ -3172,7 +3352,7 @@
         <v>36</v>
       </c>
       <c r="D96" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H96" t="s">
         <v>38</v>
@@ -3189,7 +3369,7 @@
         <v>36</v>
       </c>
       <c r="D97" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H97" t="s">
         <v>38</v>
@@ -3206,7 +3386,7 @@
         <v>36</v>
       </c>
       <c r="D98" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H98" t="s">
         <v>38</v>
@@ -3223,7 +3403,7 @@
         <v>36</v>
       </c>
       <c r="D99" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H99" t="s">
         <v>38</v>
@@ -3240,7 +3420,7 @@
         <v>36</v>
       </c>
       <c r="D100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H100" t="s">
         <v>38</v>
@@ -3257,7 +3437,7 @@
         <v>36</v>
       </c>
       <c r="D101" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H101" t="s">
         <v>38</v>
@@ -3265,16 +3445,16 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="C102" t="s">
         <v>36</v>
       </c>
       <c r="D102" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H102" t="s">
         <v>38</v>
@@ -3282,16 +3462,16 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B103" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C103" t="s">
         <v>36</v>
       </c>
       <c r="D103" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H103" t="s">
         <v>38</v>
@@ -3299,39 +3479,42 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C104" t="s">
         <v>36</v>
       </c>
       <c r="D104" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H104" t="s">
-        <v>45</v>
-      </c>
-      <c r="J104" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105" t="s">
+        <v>44</v>
+      </c>
+      <c r="C105" t="s">
+        <v>36</v>
+      </c>
+      <c r="D105" t="s">
         <v>123</v>
       </c>
-      <c r="B105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C105" t="s">
-        <v>36</v>
-      </c>
-      <c r="D105" t="s">
-        <v>122</v>
+      <c r="E105" t="s">
+        <v>45</v>
       </c>
       <c r="H105" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="J105" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -3345,7 +3528,7 @@
         <v>36</v>
       </c>
       <c r="D106" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H106" t="s">
         <v>38</v>
@@ -3362,7 +3545,7 @@
         <v>36</v>
       </c>
       <c r="D107" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H107" t="s">
         <v>38</v>
@@ -3379,7 +3562,7 @@
         <v>36</v>
       </c>
       <c r="D108" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H108" t="s">
         <v>38</v>
@@ -3396,7 +3579,7 @@
         <v>36</v>
       </c>
       <c r="D109" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H109" t="s">
         <v>38</v>
@@ -3413,7 +3596,7 @@
         <v>36</v>
       </c>
       <c r="D110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H110" t="s">
         <v>38</v>
@@ -3430,7 +3613,7 @@
         <v>36</v>
       </c>
       <c r="D111" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H111" t="s">
         <v>38</v>
@@ -3447,7 +3630,7 @@
         <v>36</v>
       </c>
       <c r="D112" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H112" t="s">
         <v>38</v>
@@ -3464,7 +3647,7 @@
         <v>36</v>
       </c>
       <c r="D113" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H113" t="s">
         <v>38</v>
@@ -3481,7 +3664,7 @@
         <v>36</v>
       </c>
       <c r="D114" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H114" t="s">
         <v>38</v>
@@ -3498,7 +3681,7 @@
         <v>36</v>
       </c>
       <c r="D115" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H115" t="s">
         <v>38</v>
@@ -3515,7 +3698,7 @@
         <v>36</v>
       </c>
       <c r="D116" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H116" t="s">
         <v>38</v>
@@ -3532,7 +3715,7 @@
         <v>36</v>
       </c>
       <c r="D117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H117" t="s">
         <v>38</v>
@@ -3549,7 +3732,7 @@
         <v>36</v>
       </c>
       <c r="D118" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H118" t="s">
         <v>38</v>
@@ -3566,7 +3749,7 @@
         <v>36</v>
       </c>
       <c r="D119" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H119" t="s">
         <v>38</v>
@@ -3583,7 +3766,7 @@
         <v>36</v>
       </c>
       <c r="D120" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H120" t="s">
         <v>38</v>
@@ -3600,7 +3783,7 @@
         <v>36</v>
       </c>
       <c r="D121" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H121" t="s">
         <v>38</v>
@@ -3617,7 +3800,7 @@
         <v>36</v>
       </c>
       <c r="D122" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H122" t="s">
         <v>38</v>
@@ -3634,7 +3817,7 @@
         <v>36</v>
       </c>
       <c r="D123" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H123" t="s">
         <v>38</v>
@@ -3651,7 +3834,7 @@
         <v>36</v>
       </c>
       <c r="D124" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H124" t="s">
         <v>38</v>
@@ -3668,7 +3851,7 @@
         <v>36</v>
       </c>
       <c r="D125" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H125" t="s">
         <v>38</v>
@@ -3685,7 +3868,7 @@
         <v>36</v>
       </c>
       <c r="D126" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H126" t="s">
         <v>38</v>
@@ -3702,7 +3885,7 @@
         <v>36</v>
       </c>
       <c r="D127" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H127" t="s">
         <v>38</v>
@@ -3710,16 +3893,16 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="B128" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="C128" t="s">
         <v>36</v>
       </c>
       <c r="D128" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H128" t="s">
         <v>38</v>
@@ -3727,16 +3910,16 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B129" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C129" t="s">
         <v>36</v>
       </c>
       <c r="D129" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="H129" t="s">
         <v>38</v>
@@ -3744,39 +3927,42 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B130" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C130" t="s">
         <v>36</v>
       </c>
       <c r="D130" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H130" t="s">
-        <v>45</v>
-      </c>
-      <c r="J130" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
+        <v>44</v>
+      </c>
+      <c r="B131" t="s">
+        <v>44</v>
+      </c>
+      <c r="C131" t="s">
+        <v>36</v>
+      </c>
+      <c r="D131" t="s">
         <v>147</v>
       </c>
-      <c r="B131" t="s">
-        <v>147</v>
-      </c>
-      <c r="C131" t="s">
-        <v>36</v>
-      </c>
-      <c r="D131" t="s">
-        <v>146</v>
+      <c r="E131" t="s">
+        <v>45</v>
       </c>
       <c r="H131" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="J131" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -3790,7 +3976,7 @@
         <v>36</v>
       </c>
       <c r="D132" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H132" t="s">
         <v>38</v>
@@ -3807,7 +3993,7 @@
         <v>36</v>
       </c>
       <c r="D133" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H133" t="s">
         <v>38</v>
@@ -3824,7 +4010,7 @@
         <v>36</v>
       </c>
       <c r="D134" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H134" t="s">
         <v>38</v>
@@ -3841,7 +4027,7 @@
         <v>36</v>
       </c>
       <c r="D135" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H135" t="s">
         <v>38</v>
@@ -3858,7 +4044,7 @@
         <v>36</v>
       </c>
       <c r="D136" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H136" t="s">
         <v>38</v>
@@ -3875,7 +4061,7 @@
         <v>36</v>
       </c>
       <c r="D137" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H137" t="s">
         <v>38</v>
@@ -3892,7 +4078,7 @@
         <v>36</v>
       </c>
       <c r="D138" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H138" t="s">
         <v>38</v>
@@ -3909,7 +4095,7 @@
         <v>36</v>
       </c>
       <c r="D139" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H139" t="s">
         <v>38</v>
@@ -3917,16 +4103,16 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="B140" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="C140" t="s">
         <v>36</v>
       </c>
       <c r="D140" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H140" t="s">
         <v>38</v>
@@ -3934,16 +4120,16 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B141" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C141" t="s">
         <v>36</v>
       </c>
       <c r="D141" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H141" t="s">
         <v>38</v>
@@ -3951,39 +4137,42 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B142" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C142" t="s">
         <v>36</v>
       </c>
       <c r="D142" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H142" t="s">
-        <v>45</v>
-      </c>
-      <c r="J142" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="1:10">
       <c r="A143" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="C143" t="s">
         <v>36</v>
       </c>
       <c r="D143" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="E143" t="s">
+        <v>45</v>
       </c>
       <c r="H143" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="J143" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -3997,7 +4186,7 @@
         <v>36</v>
       </c>
       <c r="D144" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H144" t="s">
         <v>38</v>
@@ -4005,16 +4194,16 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" t="s">
+        <v>127</v>
+      </c>
+      <c r="B145" t="s">
+        <v>127</v>
+      </c>
+      <c r="C145" t="s">
+        <v>36</v>
+      </c>
+      <c r="D145" t="s">
         <v>157</v>
-      </c>
-      <c r="B145" t="s">
-        <v>157</v>
-      </c>
-      <c r="C145" t="s">
-        <v>36</v>
-      </c>
-      <c r="D145" t="s">
-        <v>156</v>
       </c>
       <c r="H145" t="s">
         <v>38</v>
@@ -4022,16 +4211,16 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B146" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C146" t="s">
         <v>36</v>
       </c>
       <c r="D146" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H146" t="s">
         <v>38</v>
@@ -4039,16 +4228,16 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="B147" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C147" t="s">
         <v>36</v>
       </c>
       <c r="D147" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H147" t="s">
         <v>38</v>
@@ -4056,16 +4245,16 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C148" t="s">
         <v>36</v>
       </c>
       <c r="D148" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H148" t="s">
         <v>38</v>
@@ -4073,16 +4262,16 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B149" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C149" t="s">
         <v>36</v>
       </c>
       <c r="D149" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H149" t="s">
         <v>38</v>
@@ -4090,16 +4279,16 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C150" t="s">
         <v>36</v>
       </c>
       <c r="D150" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H150" t="s">
         <v>38</v>
@@ -4107,16 +4296,16 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="B151" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="C151" t="s">
         <v>36</v>
       </c>
       <c r="D151" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H151" t="s">
         <v>38</v>
@@ -4124,16 +4313,16 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B152" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C152" t="s">
         <v>36</v>
       </c>
       <c r="D152" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H152" t="s">
         <v>38</v>
@@ -4141,16 +4330,16 @@
     </row>
     <row r="153" spans="1:10">
       <c r="A153" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="B153" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="C153" t="s">
         <v>36</v>
       </c>
       <c r="D153" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H153" t="s">
         <v>38</v>
@@ -4158,16 +4347,16 @@
     </row>
     <row r="154" spans="1:10">
       <c r="A154" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B154" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C154" t="s">
         <v>36</v>
       </c>
       <c r="D154" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H154" t="s">
         <v>38</v>
@@ -4175,16 +4364,16 @@
     </row>
     <row r="155" spans="1:10">
       <c r="A155" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B155" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C155" t="s">
         <v>36</v>
       </c>
       <c r="D155" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H155" t="s">
         <v>38</v>
@@ -4192,16 +4381,16 @@
     </row>
     <row r="156" spans="1:10">
       <c r="A156" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="B156" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="C156" t="s">
         <v>36</v>
       </c>
       <c r="D156" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H156" t="s">
         <v>38</v>
@@ -4209,16 +4398,16 @@
     </row>
     <row r="157" spans="1:10">
       <c r="A157" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B157" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C157" t="s">
         <v>36</v>
       </c>
       <c r="D157" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H157" t="s">
         <v>38</v>
@@ -4226,39 +4415,42 @@
     </row>
     <row r="158" spans="1:10">
       <c r="A158" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B158" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C158" t="s">
         <v>36</v>
       </c>
       <c r="D158" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H158" t="s">
-        <v>45</v>
-      </c>
-      <c r="J158" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="159" spans="1:10">
       <c r="A159" t="s">
+        <v>44</v>
+      </c>
+      <c r="B159" t="s">
+        <v>44</v>
+      </c>
+      <c r="C159" t="s">
+        <v>36</v>
+      </c>
+      <c r="D159" t="s">
         <v>162</v>
       </c>
-      <c r="B159" t="s">
-        <v>162</v>
-      </c>
-      <c r="C159" t="s">
-        <v>36</v>
-      </c>
-      <c r="D159" t="s">
-        <v>161</v>
+      <c r="E159" t="s">
+        <v>45</v>
       </c>
       <c r="H159" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="J159" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -4272,7 +4464,7 @@
         <v>36</v>
       </c>
       <c r="D160" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H160" t="s">
         <v>38</v>
@@ -4289,7 +4481,7 @@
         <v>36</v>
       </c>
       <c r="D161" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H161" t="s">
         <v>38</v>
@@ -4306,7 +4498,7 @@
         <v>36</v>
       </c>
       <c r="D162" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H162" t="s">
         <v>38</v>
@@ -4323,7 +4515,7 @@
         <v>36</v>
       </c>
       <c r="D163" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H163" t="s">
         <v>38</v>
@@ -4340,7 +4532,7 @@
         <v>36</v>
       </c>
       <c r="D164" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H164" t="s">
         <v>38</v>
@@ -4348,16 +4540,16 @@
     </row>
     <row r="165" spans="1:10">
       <c r="A165" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="B165" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="C165" t="s">
         <v>36</v>
       </c>
       <c r="D165" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H165" t="s">
         <v>38</v>
@@ -4365,55 +4557,574 @@
     </row>
     <row r="166" spans="1:10">
       <c r="A166" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B166" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C166" t="s">
         <v>36</v>
       </c>
       <c r="D166" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H166" t="s">
-        <v>45</v>
-      </c>
-      <c r="J166" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="167" spans="1:10">
       <c r="A167" t="s">
+        <v>44</v>
+      </c>
+      <c r="B167" t="s">
+        <v>44</v>
+      </c>
+      <c r="C167" t="s">
+        <v>36</v>
+      </c>
+      <c r="D167" t="s">
+        <v>169</v>
+      </c>
+      <c r="E167" t="s">
+        <v>45</v>
+      </c>
+      <c r="H167" t="s">
         <v>46</v>
       </c>
-      <c r="B167" t="s">
+      <c r="J167" t="s">
         <v>46</v>
-      </c>
-      <c r="C167" t="s">
-        <v>36</v>
-      </c>
-      <c r="D167" t="s">
-        <v>168</v>
-      </c>
-      <c r="H167" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="168" spans="1:10">
       <c r="A168" t="s">
+        <v>47</v>
+      </c>
+      <c r="B168" t="s">
+        <v>47</v>
+      </c>
+      <c r="C168" t="s">
+        <v>36</v>
+      </c>
+      <c r="D168" t="s">
+        <v>169</v>
+      </c>
+      <c r="H168" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
+      <c r="A169" t="s">
         <v>26</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>26</v>
       </c>
-      <c r="C168" t="s">
-        <v>36</v>
-      </c>
-      <c r="D168" t="s">
-        <v>168</v>
-      </c>
-      <c r="H168" t="s">
+      <c r="C169" t="s">
+        <v>36</v>
+      </c>
+      <c r="D169" t="s">
+        <v>169</v>
+      </c>
+      <c r="H169" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
+      <c r="A170" t="s">
+        <v>44</v>
+      </c>
+      <c r="B170" t="s">
+        <v>44</v>
+      </c>
+      <c r="C170" t="s">
+        <v>36</v>
+      </c>
+      <c r="D170" t="s">
+        <v>170</v>
+      </c>
+      <c r="E170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H170" t="s">
+        <v>46</v>
+      </c>
+      <c r="J170" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
+      <c r="A171" t="s">
+        <v>47</v>
+      </c>
+      <c r="B171" t="s">
+        <v>47</v>
+      </c>
+      <c r="C171" t="s">
+        <v>36</v>
+      </c>
+      <c r="D171" t="s">
+        <v>170</v>
+      </c>
+      <c r="H171" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>171</v>
+      </c>
+      <c r="C172" t="s">
+        <v>36</v>
+      </c>
+      <c r="D172" t="s">
+        <v>170</v>
+      </c>
+      <c r="H172" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>172</v>
+      </c>
+      <c r="C173" t="s">
+        <v>36</v>
+      </c>
+      <c r="D173" t="s">
+        <v>170</v>
+      </c>
+      <c r="H173" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
+      <c r="A174" t="s">
+        <v>70</v>
+      </c>
+      <c r="B174" t="s">
+        <v>70</v>
+      </c>
+      <c r="C174" t="s">
+        <v>36</v>
+      </c>
+      <c r="D174" t="s">
+        <v>170</v>
+      </c>
+      <c r="H174" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
+      <c r="A175" t="s">
+        <v>71</v>
+      </c>
+      <c r="B175" t="s">
+        <v>71</v>
+      </c>
+      <c r="C175" t="s">
+        <v>36</v>
+      </c>
+      <c r="D175" t="s">
+        <v>170</v>
+      </c>
+      <c r="H175" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
+      <c r="A176" t="s">
+        <v>75</v>
+      </c>
+      <c r="B176" t="s">
+        <v>75</v>
+      </c>
+      <c r="C176" t="s">
+        <v>36</v>
+      </c>
+      <c r="D176" t="s">
+        <v>170</v>
+      </c>
+      <c r="H176" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
+      <c r="A177" t="s">
+        <v>76</v>
+      </c>
+      <c r="B177" t="s">
+        <v>76</v>
+      </c>
+      <c r="C177" t="s">
+        <v>36</v>
+      </c>
+      <c r="D177" t="s">
+        <v>170</v>
+      </c>
+      <c r="H177" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
+      <c r="A178" t="s">
+        <v>77</v>
+      </c>
+      <c r="B178" t="s">
+        <v>77</v>
+      </c>
+      <c r="C178" t="s">
+        <v>36</v>
+      </c>
+      <c r="D178" t="s">
+        <v>170</v>
+      </c>
+      <c r="H178" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
+      <c r="A179" t="s">
+        <v>78</v>
+      </c>
+      <c r="B179" t="s">
+        <v>78</v>
+      </c>
+      <c r="C179" t="s">
+        <v>36</v>
+      </c>
+      <c r="D179" t="s">
+        <v>170</v>
+      </c>
+      <c r="H179" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
+      <c r="A180" t="s">
+        <v>81</v>
+      </c>
+      <c r="B180" t="s">
+        <v>81</v>
+      </c>
+      <c r="C180" t="s">
+        <v>36</v>
+      </c>
+      <c r="D180" t="s">
+        <v>170</v>
+      </c>
+      <c r="H180" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" t="s">
+        <v>82</v>
+      </c>
+      <c r="B181" t="s">
+        <v>82</v>
+      </c>
+      <c r="C181" t="s">
+        <v>36</v>
+      </c>
+      <c r="D181" t="s">
+        <v>170</v>
+      </c>
+      <c r="H181" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="A182" t="s">
+        <v>83</v>
+      </c>
+      <c r="B182" t="s">
+        <v>83</v>
+      </c>
+      <c r="C182" t="s">
+        <v>36</v>
+      </c>
+      <c r="D182" t="s">
+        <v>170</v>
+      </c>
+      <c r="H182" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" t="s">
+        <v>173</v>
+      </c>
+      <c r="B183" t="s">
+        <v>173</v>
+      </c>
+      <c r="C183" t="s">
+        <v>36</v>
+      </c>
+      <c r="D183" t="s">
+        <v>170</v>
+      </c>
+      <c r="H183" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" t="s">
+        <v>174</v>
+      </c>
+      <c r="B184" t="s">
+        <v>174</v>
+      </c>
+      <c r="C184" t="s">
+        <v>36</v>
+      </c>
+      <c r="D184" t="s">
+        <v>170</v>
+      </c>
+      <c r="H184" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" t="s">
+        <v>84</v>
+      </c>
+      <c r="B185" t="s">
+        <v>84</v>
+      </c>
+      <c r="C185" t="s">
+        <v>36</v>
+      </c>
+      <c r="D185" t="s">
+        <v>170</v>
+      </c>
+      <c r="H185" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" t="s">
+        <v>85</v>
+      </c>
+      <c r="B186" t="s">
+        <v>85</v>
+      </c>
+      <c r="C186" t="s">
+        <v>36</v>
+      </c>
+      <c r="D186" t="s">
+        <v>170</v>
+      </c>
+      <c r="H186" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" t="s">
+        <v>87</v>
+      </c>
+      <c r="B187" t="s">
+        <v>87</v>
+      </c>
+      <c r="C187" t="s">
+        <v>36</v>
+      </c>
+      <c r="D187" t="s">
+        <v>170</v>
+      </c>
+      <c r="H187" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
+      <c r="A188" t="s">
+        <v>175</v>
+      </c>
+      <c r="B188" t="s">
+        <v>175</v>
+      </c>
+      <c r="C188" t="s">
+        <v>36</v>
+      </c>
+      <c r="D188" t="s">
+        <v>170</v>
+      </c>
+      <c r="H188" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" t="s">
+        <v>68</v>
+      </c>
+      <c r="B189" t="s">
+        <v>68</v>
+      </c>
+      <c r="C189" t="s">
+        <v>36</v>
+      </c>
+      <c r="D189" t="s">
+        <v>170</v>
+      </c>
+      <c r="H189" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" t="s">
+        <v>72</v>
+      </c>
+      <c r="B190" t="s">
+        <v>72</v>
+      </c>
+      <c r="C190" t="s">
+        <v>36</v>
+      </c>
+      <c r="D190" t="s">
+        <v>170</v>
+      </c>
+      <c r="H190" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" t="s">
+        <v>73</v>
+      </c>
+      <c r="B191" t="s">
+        <v>73</v>
+      </c>
+      <c r="C191" t="s">
+        <v>36</v>
+      </c>
+      <c r="D191" t="s">
+        <v>170</v>
+      </c>
+      <c r="H191" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" t="s">
+        <v>74</v>
+      </c>
+      <c r="B192" t="s">
+        <v>74</v>
+      </c>
+      <c r="C192" t="s">
+        <v>36</v>
+      </c>
+      <c r="D192" t="s">
+        <v>170</v>
+      </c>
+      <c r="H192" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" t="s">
+        <v>176</v>
+      </c>
+      <c r="B193" t="s">
+        <v>176</v>
+      </c>
+      <c r="C193" t="s">
+        <v>36</v>
+      </c>
+      <c r="D193" t="s">
+        <v>170</v>
+      </c>
+      <c r="H193" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" t="s">
+        <v>79</v>
+      </c>
+      <c r="B194" t="s">
+        <v>79</v>
+      </c>
+      <c r="C194" t="s">
+        <v>36</v>
+      </c>
+      <c r="D194" t="s">
+        <v>170</v>
+      </c>
+      <c r="H194" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" t="s">
+        <v>177</v>
+      </c>
+      <c r="B195" t="s">
+        <v>177</v>
+      </c>
+      <c r="C195" t="s">
+        <v>36</v>
+      </c>
+      <c r="D195" t="s">
+        <v>170</v>
+      </c>
+      <c r="H195" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" t="s">
+        <v>178</v>
+      </c>
+      <c r="B196" t="s">
+        <v>178</v>
+      </c>
+      <c r="C196" t="s">
+        <v>36</v>
+      </c>
+      <c r="D196" t="s">
+        <v>170</v>
+      </c>
+      <c r="H196" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" t="s">
+        <v>179</v>
+      </c>
+      <c r="B197" t="s">
+        <v>179</v>
+      </c>
+      <c r="C197" t="s">
+        <v>36</v>
+      </c>
+      <c r="D197" t="s">
+        <v>170</v>
+      </c>
+      <c r="H197" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198" t="s">
+        <v>180</v>
+      </c>
+      <c r="B198" t="s">
+        <v>180</v>
+      </c>
+      <c r="C198" t="s">
+        <v>36</v>
+      </c>
+      <c r="D198" t="s">
+        <v>170</v>
+      </c>
+      <c r="H198" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4432,67 +5143,67 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="T1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="U1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4510,31 +5221,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4573,7 +5284,7 @@
         <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -4591,16 +5302,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -4624,82 +5335,82 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="T1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="U1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="V1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="W1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="X1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Y1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Z1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4717,40 +5428,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>